<commit_message>
improvements to trends plots
</commit_message>
<xml_diff>
--- a/docs/trends-paper/wave-counts/canada-wave-counts/first_canada_wave_counts.xlsx
+++ b/docs/trends-paper/wave-counts/canada-wave-counts/first_canada_wave_counts.xlsx
@@ -383,7 +383,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>First Canada Wave</t>
+          <t>First Canada Wave (Quebec 2012)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -398,7 +398,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>First Canada Wave</t>
+          <t>First Canada Wave (Quebec 2012)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>